<commit_message>
feat: update logic, questions bank and exams bank
</commit_message>
<xml_diff>
--- a/data/pye_preguntas.xlsx
+++ b/data/pye_preguntas.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\60048007\Documents\Projects\pye\pye-evaluador-dev\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D7D2BED-AFEA-4F7B-A6FB-11EA4841DA50}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D53174F8-520F-4DA9-BEE3-A3F2EF13E855}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{C642BC87-A38A-421E-A708-FBC39335E672}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="22">
   <si>
     <t>Tipo</t>
   </si>
@@ -63,31 +63,46 @@
     <t>JSON</t>
   </si>
   <si>
-    <t>Parcial</t>
-  </si>
-  <si>
-    <t>Simulación 2° Parcial</t>
-  </si>
-  <si>
     <t>Unidad</t>
   </si>
   <si>
-    <t>V/F | OM</t>
-  </si>
-  <si>
     <t>Conceptos</t>
   </si>
   <si>
-    <t>E01</t>
-  </si>
-  <si>
-    <t>V</t>
-  </si>
-  <si>
     <t>DQ</t>
   </si>
   <si>
     <t>F</t>
+  </si>
+  <si>
+    <t>E00</t>
+  </si>
+  <si>
+    <t>Cuestionario de evaluación contínua</t>
+  </si>
+  <si>
+    <t>09/94/2025</t>
+  </si>
+  <si>
+    <t>Simulación cuestionario de evaluación contínua</t>
+  </si>
+  <si>
+    <t>Exámenes - Definición de preguntas</t>
+  </si>
+  <si>
+    <t>Exámenes - Definición</t>
+  </si>
+  <si>
+    <t>B, A, C</t>
+  </si>
+  <si>
+    <t>C, A, B</t>
+  </si>
+  <si>
+    <t>1002, 1006, 1008, 1013, 1010</t>
+  </si>
+  <si>
+    <t>2, 2, 2, 2, 2</t>
   </si>
 </sst>
 </file>
@@ -98,7 +113,7 @@
     <numFmt numFmtId="164" formatCode="0.0000"/>
     <numFmt numFmtId="165" formatCode="0.00000"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -121,8 +136,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -141,6 +164,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -154,7 +183,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -184,13 +213,22 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="16">
+  <dxfs count="17">
     <dxf>
       <font>
         <b val="0"/>
@@ -228,6 +266,45 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -247,6 +324,83 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -285,7 +439,6 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
-      <numFmt numFmtId="0" formatCode="General"/>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -369,102 +522,6 @@
         <scheme val="minor"/>
       </font>
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -524,31 +581,34 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{ED63F1EE-5662-470F-BF90-54D30B278FFD}" name="BE" displayName="BE" ref="A2:F3" totalsRowShown="0" headerRowDxfId="15" dataDxfId="14">
-  <autoFilter ref="A2:F3" xr:uid="{ED63F1EE-5662-470F-BF90-54D30B278FFD}"/>
-  <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{7E3CFFEC-1DCB-4ACB-95E8-F584ED7C7655}" name="Exámen" dataDxfId="13"/>
-    <tableColumn id="2" xr3:uid="{FFF00DC6-A32E-4402-BCA5-85199AB95AC4}" name="Tipo" dataDxfId="12"/>
-    <tableColumn id="3" xr3:uid="{8B6EAF7A-F6C1-48B3-B6DE-715DF876661F}" name="Fecha" dataDxfId="11"/>
-    <tableColumn id="4" xr3:uid="{B7392C1B-54C5-482A-A91A-6A065F8AE4FE}" name="Nombre" dataDxfId="10"/>
-    <tableColumn id="5" xr3:uid="{B28516F9-2121-4FBD-9F49-64FA0402BD87}" name="Preguntas" dataDxfId="9"/>
-    <tableColumn id="6" xr3:uid="{5AFC0726-FC65-42BE-9EDF-2A3612142BF3}" name="Puntos" dataDxfId="8"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{ED63F1EE-5662-470F-BF90-54D30B278FFD}" name="BE" displayName="BE" ref="A4:G5" totalsRowShown="0" headerRowDxfId="16" dataDxfId="15">
+  <autoFilter ref="A4:G5" xr:uid="{ED63F1EE-5662-470F-BF90-54D30B278FFD}"/>
+  <tableColumns count="7">
+    <tableColumn id="1" xr3:uid="{7E3CFFEC-1DCB-4ACB-95E8-F584ED7C7655}" name="Exámen" dataDxfId="4"/>
+    <tableColumn id="2" xr3:uid="{FFF00DC6-A32E-4402-BCA5-85199AB95AC4}" name="Tipo" dataDxfId="2"/>
+    <tableColumn id="3" xr3:uid="{8B6EAF7A-F6C1-48B3-B6DE-715DF876661F}" name="Fecha" dataDxfId="3"/>
+    <tableColumn id="4" xr3:uid="{B7392C1B-54C5-482A-A91A-6A065F8AE4FE}" name="Nombre" dataDxfId="5"/>
+    <tableColumn id="5" xr3:uid="{B28516F9-2121-4FBD-9F49-64FA0402BD87}" name="Preguntas" dataDxfId="6"/>
+    <tableColumn id="6" xr3:uid="{5AFC0726-FC65-42BE-9EDF-2A3612142BF3}" name="Puntos" dataDxfId="14"/>
+    <tableColumn id="7" xr3:uid="{1E14F2E0-3048-4916-A730-84925DDB8185}" name="JSON" dataDxfId="1">
+      <calculatedColumnFormula>"{"&amp;"id: '"&amp;A5&amp;"', type: '"&amp;B5&amp;"', name: '"&amp;D5&amp;"', date: '"&amp;C5&amp;"', questions: ["&amp;E5&amp;"], questionsPoints: ["&amp;F5&amp;"], answers: []}"&amp;IF(BE[[#This Row],[Exámen]]&lt;&gt;"",",","")</calculatedColumnFormula>
+    </tableColumn>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{D21AC528-7FB8-4E79-A187-27EE4B6442AE}" name="BE_P" displayName="BE_P" ref="A4:G8" totalsRowShown="0" headerRowDxfId="7">
-  <autoFilter ref="A4:G8" xr:uid="{D21AC528-7FB8-4E79-A187-27EE4B6442AE}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{D21AC528-7FB8-4E79-A187-27EE4B6442AE}" name="BE_P" displayName="BE_P" ref="A4:G9" totalsRowShown="0" headerRowDxfId="13">
+  <autoFilter ref="A4:G9" xr:uid="{D21AC528-7FB8-4E79-A187-27EE4B6442AE}"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{46D9BD29-77B7-4529-A1A6-FAC64F192427}" name="Exámen" dataDxfId="6"/>
-    <tableColumn id="2" xr3:uid="{75CF062F-95C4-49BE-9CF0-55BF496FDEF2}" name="Unidad" dataDxfId="5"/>
-    <tableColumn id="3" xr3:uid="{5F8039E1-D01E-43B5-BFAD-2EE69279F9DE}" name="Preguntas" dataDxfId="3"/>
-    <tableColumn id="7" xr3:uid="{10A87CDC-6113-406E-8F1C-CBEA4A4AFD38}" name="Respuesta" dataDxfId="1"/>
-    <tableColumn id="8" xr3:uid="{7A2888D8-4437-4698-9EFC-124AA27F0E63}" name="Conceptos" dataDxfId="2"/>
+    <tableColumn id="1" xr3:uid="{46D9BD29-77B7-4529-A1A6-FAC64F192427}" name="Exámen" dataDxfId="12"/>
+    <tableColumn id="2" xr3:uid="{75CF062F-95C4-49BE-9CF0-55BF496FDEF2}" name="Unidad" dataDxfId="11"/>
+    <tableColumn id="3" xr3:uid="{5F8039E1-D01E-43B5-BFAD-2EE69279F9DE}" name="Preguntas" dataDxfId="10"/>
+    <tableColumn id="7" xr3:uid="{10A87CDC-6113-406E-8F1C-CBEA4A4AFD38}" name="Respuesta" dataDxfId="9"/>
+    <tableColumn id="8" xr3:uid="{7A2888D8-4437-4698-9EFC-124AA27F0E63}" name="Conceptos" dataDxfId="8"/>
     <tableColumn id="4" xr3:uid="{7B8D6CC9-E181-464B-B61F-4A34B336F909}" name="Puntos" dataDxfId="0"/>
-    <tableColumn id="9" xr3:uid="{267A0D78-7694-40DF-822F-171970B3B11E}" name="DQ" dataDxfId="4">
+    <tableColumn id="9" xr3:uid="{267A0D78-7694-40DF-822F-171970B3B11E}" name="DQ" dataDxfId="7">
       <calculatedColumnFormula>COUNTIF(BE_P[Preguntas],BE_P[[#This Row],[Preguntas]])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -854,74 +914,86 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CD84005E-B40E-4AB3-A398-3CB8B8F0029B}">
   <sheetPr codeName="Sheet5"/>
-  <dimension ref="A1:H3"/>
+  <dimension ref="A1:I5"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="4" topLeftCell="B5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="A3" sqref="A3"/>
+      <selection pane="bottomRight" activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="24" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.77734375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="8.88671875" style="1"/>
-    <col min="3" max="3" width="10.5546875" style="5" customWidth="1"/>
-    <col min="4" max="4" width="24.5546875" style="1" customWidth="1"/>
-    <col min="5" max="6" width="25.77734375" style="1" customWidth="1"/>
-    <col min="7" max="7" width="8.88671875" style="1"/>
-    <col min="8" max="8" width="52.6640625" style="1" customWidth="1"/>
-    <col min="9" max="16384" width="8.88671875" style="1"/>
+    <col min="1" max="1" width="11.44140625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="25.77734375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="11.77734375" style="5" customWidth="1"/>
+    <col min="4" max="7" width="25.77734375" style="1" customWidth="1"/>
+    <col min="8" max="8" width="8.88671875" style="1"/>
+    <col min="9" max="9" width="52.6640625" style="1" customWidth="1"/>
+    <col min="10" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="12" t="s">
+        <v>17</v>
+      </c>
       <c r="C1" s="1"/>
     </row>
-    <row r="2" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="3" t="s">
+    <row r="2" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C2" s="1"/>
+    </row>
+    <row r="3" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C3" s="1"/>
+    </row>
+    <row r="4" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B4" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C4" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D4" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="E4" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="F4" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="H2" s="3" t="s">
+      <c r="G4" s="3" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="2" t="s">
+      <c r="I4" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E3" s="1" t="e">
-        <f>"["&amp;_xlfn.CONCAT(BE_P!#REF!)&amp;"]"</f>
-        <v>#REF!</v>
-      </c>
-      <c r="F3" s="1" t="e">
-        <f>"["&amp;_xlfn.CONCAT(BE_P!#REF!)&amp;"]"</f>
-        <v>#REF!</v>
-      </c>
-      <c r="H3" s="1" t="e">
-        <f>"{"&amp;"id: '"&amp;A3&amp;"', type: '"&amp;B3&amp;"', name: '"&amp;D3&amp;"', date: '"&amp;C3&amp;"', questions: "&amp;E3&amp;", questionsPoints: "&amp;F3&amp;", answers: []}"&amp;IF(#REF!&lt;&gt;"",",","")</f>
-        <v>#REF!</v>
+      <c r="C5" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D5" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="G5" s="1" t="str">
+        <f>"{"&amp;"id: '"&amp;A5&amp;"', type: '"&amp;B5&amp;"', name: '"&amp;D5&amp;"', date: '"&amp;C5&amp;"', questions: ["&amp;E5&amp;"], questionsPoints: ["&amp;F5&amp;"], answers: []}"&amp;IF(BE[[#This Row],[Exámen]]&lt;&gt;"",",","")</f>
+        <v>{id: 'E00', type: 'Cuestionario de evaluación contínua', name: 'Simulación cuestionario de evaluación contínua', date: '09/94/2025', questions: [1002, 1006, 1008, 1013, 1010], questionsPoints: [2, 2, 2, 2, 2], answers: []},</v>
       </c>
     </row>
   </sheetData>
@@ -936,13 +1008,13 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3F3D13BB-70E6-4209-BE45-5D6C0D3E5EFB}">
   <sheetPr codeName="Sheet6"/>
-  <dimension ref="A1:G8"/>
+  <dimension ref="A1:G9"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
       <pane xSplit="1" ySplit="4" topLeftCell="B5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="A5" sqref="A5"/>
+      <selection pane="bottomRight" activeCell="C5" sqref="C5:C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -957,13 +1029,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="1"/>
-      <c r="B1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C1" s="1">
-        <v>0.22222</v>
-      </c>
+      <c r="A1" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
       <c r="D1" s="8"/>
       <c r="F1" s="1"/>
     </row>
@@ -977,12 +1047,12 @@
     <row r="3" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="6">
         <f>SUBTOTAL(3,BE_P[Exámen])</f>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B3" s="8"/>
       <c r="C3" s="6">
         <f>SUBTOTAL(3,BE_P[Preguntas])</f>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D3" s="8"/>
       <c r="F3" s="7">
@@ -995,7 +1065,7 @@
         <v>4</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>2</v>
@@ -1004,30 +1074,30 @@
         <v>1</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="F4" s="3" t="s">
         <v>3</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B5" s="2">
         <v>1</v>
       </c>
       <c r="C5" s="2">
-        <v>1001</v>
+        <v>1002</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="F5" s="4">
-        <v>2.5</v>
+        <v>2</v>
       </c>
       <c r="G5" s="2">
         <f>COUNTIF(BE_P[Preguntas],BE_P[[#This Row],[Preguntas]])</f>
@@ -1036,19 +1106,19 @@
     </row>
     <row r="6" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B6" s="2">
         <v>1</v>
       </c>
       <c r="C6" s="2">
-        <v>1002</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>16</v>
+        <v>1006</v>
+      </c>
+      <c r="D6" s="2">
+        <v>2</v>
       </c>
       <c r="F6" s="4">
-        <v>2.5</v>
+        <v>2</v>
       </c>
       <c r="G6" s="10">
         <f>COUNTIF(BE_P[Preguntas],BE_P[[#This Row],[Preguntas]])</f>
@@ -1057,19 +1127,19 @@
     </row>
     <row r="7" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B7" s="2">
         <v>1</v>
       </c>
       <c r="C7" s="2">
-        <v>1003</v>
+        <v>1008</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="F7" s="4">
-        <v>2.5</v>
+        <v>2</v>
       </c>
       <c r="G7" s="10">
         <f>COUNTIF(BE_P[Preguntas],BE_P[[#This Row],[Preguntas]])</f>
@@ -1078,21 +1148,42 @@
     </row>
     <row r="8" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B8" s="2">
         <v>1</v>
       </c>
       <c r="C8" s="2">
-        <v>1004</v>
+        <v>1013</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="F8" s="4">
-        <v>2.5</v>
+        <v>2</v>
       </c>
       <c r="G8" s="10">
+        <f>COUNTIF(BE_P[Preguntas],BE_P[[#This Row],[Preguntas]])</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B9" s="2">
+        <v>1</v>
+      </c>
+      <c r="C9" s="2">
+        <v>1010</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F9" s="4">
+        <v>2</v>
+      </c>
+      <c r="G9" s="10">
         <f>COUNTIF(BE_P[Preguntas],BE_P[[#This Row],[Preguntas]])</f>
         <v>1</v>
       </c>

</xml_diff>